<commit_message>
add dept by superadmin inside add employee
</commit_message>
<xml_diff>
--- a/superadmin/PHPExcel/employeeData.xlsx
+++ b/superadmin/PHPExcel/employeeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\mygatecutm\superadmin\PHPExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F26DC4D-DD57-4FCF-AE8F-F66DD53D017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE614671-D83E-46C4-AA66-6E991FCE6EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{743BF52B-2C3A-4DC4-A3A6-ECE32DFE79A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>BBSR</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>chinmayakumarbiswal16045@gmail.com</t>
+  </si>
+  <si>
+    <t>Emp Dept</t>
+  </si>
+  <si>
+    <t>IT Admin</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,10 +462,12 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -481,6 +489,9 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="3"/>

</xml_diff>